<commit_message>
Update to LDA data processing
</commit_message>
<xml_diff>
--- a/LDA_model/LDA_hyperparameter_tuning.xlsx
+++ b/LDA_model/LDA_hyperparameter_tuning.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jia Kai\Desktop\ECE324_Introduction_To_Machine_Intelligence\00 Project REScipe\public_repo\REScipe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jia Kai\Desktop\ECE324_Introduction_To_Machine_Intelligence\00 Project REScipe\public_repo\REScipe\LDA_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A297EC88-8EBB-44BA-8EE5-A04C5226319F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A678E52-75AE-4E02-B728-627944CA36C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A82F6BC3-A158-4978-8193-4B73B6813A13}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t>Chunk#</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>90 (158s)</t>
+  </si>
+  <si>
+    <t>passes</t>
   </si>
 </sst>
 </file>
@@ -273,7 +276,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -313,6 +316,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -363,9 +372,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -384,9 +390,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -455,7 +458,13 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -774,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{237D5539-4799-4441-AE7D-16038BC0F9BC}">
   <dimension ref="A1:U45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -808,16 +817,16 @@
       <c r="F1">
         <v>8</v>
       </c>
-      <c r="G1" s="14">
+      <c r="G1" s="12">
         <v>16</v>
       </c>
-      <c r="H1" s="14">
+      <c r="H1" s="12">
         <v>32</v>
       </c>
-      <c r="I1" s="14">
+      <c r="I1" s="12">
         <v>64</v>
       </c>
-      <c r="J1" s="14"/>
+      <c r="J1" s="12"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -826,170 +835,170 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>100</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11" t="s">
+      <c r="D3" s="10"/>
+      <c r="E3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="2" t="s">
+      <c r="J3" s="12"/>
+      <c r="K3" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>150</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="14"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>200</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="14"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>250</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="13" t="s">
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="14"/>
+      <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>300</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="31" t="s">
+      <c r="I7" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="14"/>
+      <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>350</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="20" t="s">
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="30" t="s">
+      <c r="I8" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="14"/>
+      <c r="J8" s="12"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>400</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="32" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="33" t="s">
+      <c r="I9" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="14"/>
+      <c r="J9" s="12"/>
     </row>
     <row r="10" spans="1:17" ht="18" x14ac:dyDescent="0.35">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
@@ -998,16 +1007,16 @@
       <c r="F12" t="s">
         <v>0</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="12">
         <v>16</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="12">
         <v>32</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="12">
         <v>64</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="12">
         <v>128</v>
       </c>
       <c r="K12">
@@ -1024,16 +1033,16 @@
       <c r="F13" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="12">
         <v>32</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="12">
         <v>16</v>
       </c>
-      <c r="I13" s="14">
+      <c r="I13" s="12">
         <v>8</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="12">
         <v>4</v>
       </c>
       <c r="K13">
@@ -1041,20 +1050,23 @@
       </c>
       <c r="L13" s="1">
         <v>1</v>
+      </c>
+      <c r="M13" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E14">
         <v>100</v>
       </c>
-      <c r="G14" s="20"/>
-      <c r="H14" s="29" t="s">
+      <c r="G14" s="18"/>
+      <c r="H14" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="20"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11" t="s">
+      <c r="I14" s="18"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1062,27 +1074,27 @@
       <c r="E15">
         <v>150</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E16">
         <v>200</v>
       </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="15" t="s">
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="29" t="s">
+      <c r="K16" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="L16" s="30" t="s">
+      <c r="L16" s="28" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1090,112 +1102,112 @@
       <c r="E17">
         <v>250</v>
       </c>
-      <c r="G17" s="13"/>
-      <c r="H17" s="19" t="s">
+      <c r="G17" s="11"/>
+      <c r="H17" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="J17" s="15"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
     </row>
     <row r="18" spans="4:21" x14ac:dyDescent="0.3">
       <c r="E18">
         <v>300</v>
       </c>
-      <c r="G18" s="18" t="s">
+      <c r="G18" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="H18" s="34" t="s">
+      <c r="H18" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="I18" s="35" t="s">
+      <c r="I18" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="J18" s="37" t="s">
+      <c r="J18" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
     </row>
     <row r="19" spans="4:21" x14ac:dyDescent="0.3">
       <c r="E19">
         <v>350</v>
       </c>
-      <c r="G19" s="20"/>
-      <c r="H19" s="29" t="s">
+      <c r="G19" s="18"/>
+      <c r="H19" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="I19" s="33" t="s">
+      <c r="I19" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="J19" s="21"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
     </row>
     <row r="20" spans="4:21" x14ac:dyDescent="0.3">
       <c r="E20">
         <v>400</v>
       </c>
-      <c r="G20" s="23"/>
-      <c r="H20" s="36" t="s">
+      <c r="G20" s="21"/>
+      <c r="H20" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="I20" s="30" t="s">
+      <c r="I20" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="J20" s="21"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="10" t="s">
+      <c r="J20" s="19"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="4:21" ht="18" x14ac:dyDescent="0.35">
-      <c r="G21" s="16"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="N21" s="2" t="s">
+      <c r="G21" s="14"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="N21" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2"/>
-      <c r="U21" s="3"/>
+      <c r="O21" s="35"/>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="35"/>
+      <c r="S21" s="35"/>
+      <c r="T21" s="35"/>
+      <c r="U21" s="2"/>
     </row>
     <row r="22" spans="4:21" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
+      <c r="F22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
     </row>
     <row r="23" spans="4:21" x14ac:dyDescent="0.3">
       <c r="E23" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="12" t="s">
         <v>0</v>
       </c>
       <c r="G23">
         <v>64</v>
       </c>
-      <c r="H23" s="14">
+      <c r="H23" s="12">
         <v>32</v>
       </c>
-      <c r="I23" s="14">
+      <c r="I23" s="12">
         <v>64</v>
       </c>
-      <c r="J23" s="14">
+      <c r="J23" s="12">
         <v>128</v>
       </c>
       <c r="K23">
@@ -1218,19 +1230,19 @@
       <c r="E24" t="s">
         <v>2</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="12" t="s">
         <v>3</v>
       </c>
       <c r="G24">
         <v>256</v>
       </c>
-      <c r="H24" s="14">
+      <c r="H24" s="12">
         <v>128</v>
       </c>
-      <c r="I24" s="14">
+      <c r="I24" s="12">
         <v>64</v>
       </c>
-      <c r="J24" s="14">
+      <c r="J24" s="12">
         <v>32</v>
       </c>
       <c r="K24">
@@ -1247,58 +1259,61 @@
       </c>
       <c r="O24" s="1">
         <v>1</v>
+      </c>
+      <c r="P24" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="4:21" x14ac:dyDescent="0.3">
       <c r="E25">
         <v>100</v>
       </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
     </row>
     <row r="26" spans="4:21" x14ac:dyDescent="0.3">
       <c r="E26">
         <v>150</v>
       </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
     </row>
     <row r="27" spans="4:21" x14ac:dyDescent="0.3">
       <c r="E27">
         <v>200</v>
       </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="28" t="s">
+      <c r="F27" s="12"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="L27" s="30" t="s">
+      <c r="L27" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="M27" s="25"/>
-      <c r="N27" s="24" t="s">
+      <c r="M27" s="23"/>
+      <c r="N27" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="O27" s="24" t="s">
+      <c r="O27" s="22" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1306,65 +1321,65 @@
       <c r="E28">
         <v>250</v>
       </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
-      <c r="M28" s="25"/>
-      <c r="N28" s="26"/>
-      <c r="O28" s="26"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="24"/>
     </row>
     <row r="29" spans="4:21" x14ac:dyDescent="0.3">
       <c r="E29">
         <v>300</v>
       </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="22" t="s">
+      <c r="F29" s="12"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="I29" s="19"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
     </row>
     <row r="30" spans="4:21" x14ac:dyDescent="0.3">
       <c r="E30">
         <v>350</v>
       </c>
-      <c r="F30" s="14"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="30" t="s">
+      <c r="F30" s="12"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="J30" s="20"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
     </row>
     <row r="31" spans="4:21" x14ac:dyDescent="0.3">
       <c r="E31">
         <v>400</v>
       </c>
-      <c r="F31" s="14"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
     </row>
     <row r="35" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K35" s="1"/>
@@ -1401,79 +1416,79 @@
     </row>
     <row r="38" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K38" s="1"/>
-      <c r="L38" s="5"/>
-      <c r="M38" s="5"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="6"/>
-      <c r="S38" s="5"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="5"/>
+      <c r="S38" s="4"/>
     </row>
     <row r="39" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K39" s="1"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="6"/>
-      <c r="O39" s="6"/>
-      <c r="P39" s="6"/>
-      <c r="Q39" s="6"/>
-      <c r="R39" s="6"/>
-      <c r="S39" s="5"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="5"/>
+      <c r="R39" s="5"/>
+      <c r="S39" s="4"/>
     </row>
     <row r="40" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K40" s="1"/>
-      <c r="L40" s="5"/>
-      <c r="M40" s="5"/>
-      <c r="N40" s="6"/>
-      <c r="O40" s="6"/>
-      <c r="P40" s="6"/>
-      <c r="Q40" s="6"/>
-      <c r="R40" s="6"/>
-      <c r="S40" s="5"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+      <c r="P40" s="5"/>
+      <c r="Q40" s="5"/>
+      <c r="R40" s="5"/>
+      <c r="S40" s="4"/>
     </row>
     <row r="41" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K41" s="1"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
-      <c r="N41" s="6"/>
-      <c r="O41" s="6"/>
-      <c r="P41" s="6"/>
-      <c r="Q41" s="6"/>
-      <c r="R41" s="6"/>
-      <c r="S41" s="5"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="5"/>
+      <c r="R41" s="5"/>
+      <c r="S41" s="4"/>
     </row>
     <row r="42" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K42" s="1"/>
-      <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
-      <c r="N42" s="6"/>
-      <c r="O42" s="6"/>
-      <c r="P42" s="6"/>
-      <c r="Q42" s="6"/>
-      <c r="R42" s="6"/>
-      <c r="S42" s="5"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5"/>
+      <c r="S42" s="4"/>
     </row>
     <row r="43" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K43" s="1"/>
-      <c r="L43" s="5"/>
-      <c r="M43" s="5"/>
-      <c r="N43" s="6"/>
-      <c r="O43" s="6"/>
-      <c r="P43" s="6"/>
-      <c r="Q43" s="6"/>
-      <c r="R43" s="6"/>
-      <c r="S43" s="5"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+      <c r="Q43" s="5"/>
+      <c r="R43" s="5"/>
+      <c r="S43" s="4"/>
     </row>
     <row r="44" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-      <c r="P44" s="4"/>
-      <c r="Q44" s="4"/>
-      <c r="R44" s="4"/>
+      <c r="N44" s="3"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="3"/>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
       <c r="S44" s="1"/>
     </row>
     <row r="45" spans="11:19" x14ac:dyDescent="0.3">

</xml_diff>